<commit_message>
back to Cp simplification
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-60" windowWidth="29040" windowHeight="15780"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -460,11 +460,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="149919360"/>
-        <c:axId val="149919936"/>
+        <c:axId val="82105984"/>
+        <c:axId val="82106560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149919360"/>
+        <c:axId val="82105984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -560,13 +560,13 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149919936"/>
+        <c:crossAx val="82106560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149919936"/>
+        <c:axId val="82106560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +660,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="149919360"/>
+        <c:crossAx val="82105984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1027,11 +1027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89374720"/>
-        <c:axId val="89375296"/>
+        <c:axId val="59596800"/>
+        <c:axId val="59597376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89374720"/>
+        <c:axId val="59596800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1127,13 +1127,13 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89375296"/>
+        <c:crossAx val="59597376"/>
         <c:crossesAt val="-200"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89375296"/>
+        <c:axId val="59597376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1227,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89374720"/>
+        <c:crossAx val="59596800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1594,11 +1594,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89377024"/>
-        <c:axId val="89377600"/>
+        <c:axId val="59599104"/>
+        <c:axId val="59599680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89377024"/>
+        <c:axId val="59599104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1694,13 +1694,13 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89377600"/>
+        <c:crossAx val="59599680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89377600"/>
+        <c:axId val="59599680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1794,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89377024"/>
+        <c:crossAx val="59599104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3928,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32:O43"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S61" sqref="S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6001,13 +6001,13 @@
       <c r="AF32" t="s">
         <v>30</v>
       </c>
-      <c r="AG32" t="str">
-        <f>_xlfn.CONCAT(V32:Z32)</f>
-        <v>Lj0[1] := 13.5002998339463;</v>
-      </c>
-      <c r="AH32" t="str">
-        <f>_xlfn.CONCAT(AB32:AF32)</f>
-        <v>Vj0[1] := 2.77418258346388E-21;</v>
+      <c r="AG32" t="e">
+        <f ca="1">_xlfn.CONCAT(V32:Z32)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH32" t="e">
+        <f ca="1">_xlfn.CONCAT(AB32:AF32)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="33" spans="2:34" x14ac:dyDescent="0.25">
@@ -6080,13 +6080,13 @@
       <c r="AF33" t="s">
         <v>30</v>
       </c>
-      <c r="AG33" t="str">
-        <f t="shared" ref="AG33:AG43" si="4">_xlfn.CONCAT(V33:Z33)</f>
-        <v>Lj0[2] := 20.737343306693;</v>
-      </c>
-      <c r="AH33" t="str">
-        <f t="shared" ref="AH33:AH43" si="5">_xlfn.CONCAT(AB33:AF33)</f>
-        <v>Vj0[2] := 18.0003468852498;</v>
+      <c r="AG33" t="e">
+        <f t="shared" ref="AG33:AG43" ca="1" si="4">_xlfn.CONCAT(V33:Z33)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH33" t="e">
+        <f t="shared" ref="AH33:AH43" ca="1" si="5">_xlfn.CONCAT(AB33:AF33)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="34" spans="2:34" x14ac:dyDescent="0.25">
@@ -6159,13 +6159,13 @@
       <c r="AF34" t="s">
         <v>30</v>
       </c>
-      <c r="AG34" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[3] := 20.9287009858463;</v>
-      </c>
-      <c r="AH34" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[3] := 25.2373903579965;</v>
+      <c r="AG34" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH34" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="35" spans="2:34" x14ac:dyDescent="0.25">
@@ -6238,13 +6238,13 @@
       <c r="AF35" t="s">
         <v>30</v>
       </c>
-      <c r="AG35" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[4] := 19.550301112881;</v>
-      </c>
-      <c r="AH35" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[4] := 25.4287480371498;</v>
+      <c r="AG35" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH35" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="36" spans="2:34" x14ac:dyDescent="0.25">
@@ -6317,13 +6317,13 @@
       <c r="AF36" t="s">
         <v>30</v>
       </c>
-      <c r="AG36" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[5] := 26.0363992148964;</v>
-      </c>
-      <c r="AH36" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[5] := 24.0503481641846;</v>
+      <c r="AG36" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH36" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="37" spans="2:34" x14ac:dyDescent="0.25">
@@ -6396,13 +6396,13 @@
       <c r="AF37" t="s">
         <v>30</v>
       </c>
-      <c r="AG37" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[6] := 26.2070994939306;</v>
-      </c>
-      <c r="AH37" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[6] := 16.7362405377912;</v>
+      <c r="AG37" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH37" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="38" spans="2:34" x14ac:dyDescent="0.25">
@@ -6475,13 +6475,13 @@
       <c r="AF38" t="s">
         <v>30</v>
       </c>
-      <c r="AG38" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[7] := 26.116418529036;</v>
-      </c>
-      <c r="AH38" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[7] := 16.9069408168254;</v>
+      <c r="AG38" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH38" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="39" spans="2:34" x14ac:dyDescent="0.25">
@@ -6554,13 +6554,13 @@
       <c r="AF39" t="s">
         <v>30</v>
       </c>
-      <c r="AG39" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[8] := 26.0990899732481;</v>
-      </c>
-      <c r="AH39" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[8] := 16.8162598519308;</v>
+      <c r="AG39" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH39" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="40" spans="2:34" x14ac:dyDescent="0.25">
@@ -6633,13 +6633,13 @@
       <c r="AF40" t="s">
         <v>30</v>
       </c>
-      <c r="AG40" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[9] := 26.2015883534268;</v>
-      </c>
-      <c r="AH40" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[9] := 16.7989312961429;</v>
+      <c r="AG40" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH40" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="41" spans="2:34" x14ac:dyDescent="0.25">
@@ -6710,13 +6710,13 @@
       <c r="AF41" t="s">
         <v>30</v>
       </c>
-      <c r="AG41" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[10] := 26.1897968366788;</v>
-      </c>
-      <c r="AH41" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[10] := 16.9014296763216;</v>
+      <c r="AG41" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH41" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="42" spans="2:34" x14ac:dyDescent="0.25">
@@ -6787,13 +6787,13 @@
       <c r="AF42" t="s">
         <v>30</v>
       </c>
-      <c r="AG42" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[11] := 25.511424209471;</v>
-      </c>
-      <c r="AH42" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[11] := 16.8896381595736;</v>
+      <c r="AG42" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH42" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="43" spans="2:34" x14ac:dyDescent="0.25">
@@ -6864,13 +6864,13 @@
       <c r="AF43" t="s">
         <v>30</v>
       </c>
-      <c r="AG43" t="str">
-        <f t="shared" si="4"/>
-        <v>Lj0[12] := 9.30015867710519;</v>
-      </c>
-      <c r="AH43" t="str">
-        <f t="shared" si="5"/>
-        <v>Vj0[12] := 16.2112655323659;</v>
+      <c r="AG43" t="e">
+        <f t="shared" ca="1" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="AH43" t="e">
+        <f t="shared" ca="1" si="5"/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="46" spans="2:34" x14ac:dyDescent="0.25">

</xml_diff>